<commit_message>
Added LivingWill profiles and example
</commit_message>
<xml_diff>
--- a/Mappings/LivingWill - STU3.xlsx
+++ b/Mappings/LivingWill - STU3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t xml:space="preserve">Zorginformatiebouwsteen – BGZ  </t>
   </si>
@@ -194,13 +194,19 @@
     <t>Anders</t>
   </si>
   <si>
-    <t>No note or comment element available</t>
-  </si>
-  <si>
     <t xml:space="preserve">Consent  </t>
   </si>
   <si>
     <t>No reference available to a Condition resource. Ask Micheal why this concept is needed in the ZIB.</t>
+  </si>
+  <si>
+    <t>Modeling question: leave it open? e.g. Source[X]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be more open with regard to references (Patient/Practitioner/Organization)? </t>
+  </si>
+  <si>
+    <t>No note or comment element available - gForge #13313</t>
   </si>
 </sst>
 </file>
@@ -871,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -920,7 +926,7 @@
       <c r="H2" s="39"/>
       <c r="I2" s="40"/>
       <c r="J2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -991,7 +997,9 @@
       <c r="J5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="32"/>
+      <c r="K5" s="32" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="18">
@@ -1014,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.5">
@@ -1039,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1063,7 +1071,9 @@
       <c r="J8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="26" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>